<commit_message>
updated models and UI to support correct importing and exporting of excel files for Product_Type, Product_Size, Product_Name, and Product. Also updated the demo excel files to work correctly with the new models
</commit_message>
<xml_diff>
--- a/addons/pharma-pos/demo_excel/pharma_pos.product_size.xlsx
+++ b/addons/pharma-pos/demo_excel/pharma_pos.product_size.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Product Size</t>
   </si>
@@ -28,13 +28,16 @@
     <t>500 ml</t>
   </si>
   <si>
-    <t>Bottle</t>
+    <t>Tablet</t>
   </si>
   <si>
     <t>10 mg</t>
   </si>
   <si>
-    <t>Tablet</t>
+    <t>20 cc</t>
+  </si>
+  <si>
+    <t>Injection</t>
   </si>
 </sst>
 </file>
@@ -384,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,10 +423,21 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3">
         <v>44225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>